<commit_message>
Tcc  dia 10072018 atualizado
</commit_message>
<xml_diff>
--- a/Tcc 1 2ª Tentativa/Disciplinasecódigos.xlsx
+++ b/Tcc 1 2ª Tentativa/Disciplinasecódigos.xlsx
@@ -16,14 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Disciplinas</t>
   </si>
   <si>
-    <t xml:space="preserve">Código </t>
-  </si>
-  <si>
     <t xml:space="preserve">Fundamentos de Sistemas de Informação </t>
   </si>
   <si>
@@ -214,6 +211,21 @@
   </si>
   <si>
     <t>COM032</t>
+  </si>
+  <si>
+    <t>Código</t>
+  </si>
+  <si>
+    <t>Algoritmos e estrutura de dados II</t>
+  </si>
+  <si>
+    <t>Algoritmos e estrutura de dados III</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sistemas Operacionais </t>
+  </si>
+  <si>
+    <t>Linguagens de Programação</t>
   </si>
 </sst>
 </file>
@@ -263,6 +275,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:B37" totalsRowShown="0">
+  <autoFilter ref="A1:B37"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Disciplinas"/>
+    <tableColumn id="2" name="Código"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -552,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,267 +592,290 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
         <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
         <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
         <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
         <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
         <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
         <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
         <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
         <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
         <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
         <v>34</v>
-      </c>
-      <c r="B18" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
         <v>36</v>
-      </c>
-      <c r="B19" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s">
         <v>38</v>
-      </c>
-      <c r="B20" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" t="s">
         <v>40</v>
-      </c>
-      <c r="B21" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
         <v>42</v>
-      </c>
-      <c r="B22" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" t="s">
         <v>44</v>
-      </c>
-      <c r="B23" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
         <v>46</v>
-      </c>
-      <c r="B24" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" t="s">
         <v>48</v>
-      </c>
-      <c r="B25" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" t="s">
         <v>50</v>
-      </c>
-      <c r="B26" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" t="s">
         <v>52</v>
-      </c>
-      <c r="B27" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" t="s">
         <v>56</v>
-      </c>
-      <c r="B29" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" t="s">
         <v>58</v>
-      </c>
-      <c r="B30" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" t="s">
         <v>60</v>
-      </c>
-      <c r="B31" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" t="s">
         <v>62</v>
-      </c>
-      <c r="B32" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" t="s">
         <v>64</v>
       </c>
-      <c r="B33" t="s">
-        <v>65</v>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>